<commit_message>
Made web app fully responsive with mobile-first design
</commit_message>
<xml_diff>
--- a/data/qr_validation_tracker.xlsx
+++ b/data/qr_validation_tracker.xlsx
@@ -559,25 +559,39 @@
           <t>Factory_Reached</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-04-06 20:58:58</t>
+          <t>2025-04-07 14:54:30</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>28.6548,77.1871</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+          <t>28.507719,77.373215</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Dealer_Reached</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025-04-07 15:22:30</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>28.507874,77.372948</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
@@ -611,10 +625,8 @@
           <t>Factory_Reached</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F3" t="n">
+        <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Updated QR code validation with improved image handling and responsive design
</commit_message>
<xml_diff>
--- a/data/qr_validation_tracker.xlsx
+++ b/data/qr_validation_tracker.xlsx
@@ -554,48 +554,34 @@
       <c r="D2" t="n">
         <v>3096004441</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Factory_Reached</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-04-07 14:54:30</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>28.507719,77.373215</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Dealer_Reached</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2025-04-07 15:22:30</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>28.507874,77.372948</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Retailer_Reached</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2025-04-07 17:30:18</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
@@ -620,24 +606,10 @@
       <c r="D3" t="n">
         <v>3096004441</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Factory_Reached</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-04-06 20:58:58</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>28.6548,77.1871</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>

</xml_diff>

<commit_message>
Fixed tracker route to handle guest access properly
</commit_message>
<xml_diff>
--- a/data/qr_validation_tracker.xlsx
+++ b/data/qr_validation_tracker.xlsx
@@ -554,10 +554,26 @@
       <c r="D2" t="n">
         <v>3096004441</v>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Factory_Reached</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-04-07 17:54:30</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -567,14 +583,12 @@
           <t>Retailer_Reached</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="N2" t="n">
+        <v>3</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2025-04-07 17:30:18</t>
+          <t>2025-04-07 17:47:40</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">

</xml_diff>

<commit_message>
Fixed reports route and added location updates for QR validation
</commit_message>
<xml_diff>
--- a/data/qr_validation_tracker.xlsx
+++ b/data/qr_validation_tracker.xlsx
@@ -559,14 +559,12 @@
           <t>Factory_Reached</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-04-07 17:54:30</t>
+          <t>2025-04-07 18:11:05</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -574,10 +572,24 @@
           <t>Location not available</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Dealer_Reached</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025-04-07 18:12:03</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>Retailer_Reached</t>
@@ -588,7 +600,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2025-04-07 17:47:40</t>
+          <t>2025-04-07 18:17:44</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -597,9 +609,21 @@
         </is>
       </c>
       <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>2025-04-07 18:24:28</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Factory_Reached</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -620,22 +644,62 @@
       <c r="D3" t="n">
         <v>3096004441</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Factory_Reached</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-04-07 18:11:05</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Dealer_Reached</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2025-04-07 18:12:03</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>2025-04-07 18:15:15</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Factory_Reached</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -656,10 +720,24 @@
       <c r="D4" t="n">
         <v>3096004441</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Factory_Reached</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-04-07 18:11:05</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -669,9 +747,21 @@
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>2025-04-07 18:10:33</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Factory_Reached</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -692,10 +782,24 @@
       <c r="D5" t="n">
         <v>3096004441</v>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Factory_Reached</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-04-07 18:11:05</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -705,9 +809,21 @@
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>2025-04-07 18:10:33</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Location not available</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Factory_Reached</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">

</xml_diff>